<commit_message>
feat(ld46) update card definitions
</commit_message>
<xml_diff>
--- a/packages/ld46/docs/cards/Characters.xlsx
+++ b/packages/ld46/docs/cards/Characters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\jou\packages\ld46\docs\cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69131345-A619-4597-868F-5AFF6928CE97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1A9D84-33FA-4F2F-A962-CB245D27D8E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="129">
   <si>
     <t>level</t>
   </si>
@@ -62,9 +62,6 @@
     <t>cp</t>
   </si>
   <si>
-    <t>excitement</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -227,9 +224,6 @@
     <t>-3 creature CP</t>
   </si>
   <si>
-    <t>+3 creature CP when fighting with Kephissa</t>
-  </si>
-  <si>
     <t>Vibenia</t>
   </si>
   <si>
@@ -242,9 +236,6 @@
     <t>"MAXIMUS! MAXIMUS!" Roars the crowd</t>
   </si>
   <si>
-    <t>+2 Excitement per fight</t>
-  </si>
-  <si>
     <t>Spear</t>
   </si>
   <si>
@@ -263,156 +254,181 @@
     <t>Traex</t>
   </si>
   <si>
-    <t>-5 creature CP</t>
-  </si>
-  <si>
-    <t>-7 creature CP</t>
-  </si>
-  <si>
-    <t>-6 creature CP</t>
-  </si>
-  <si>
     <t>Net</t>
   </si>
   <si>
+    <t>Short Sword</t>
+  </si>
+  <si>
+    <t>Equite</t>
+  </si>
+  <si>
+    <t>+5 CP when fighting SLOW</t>
+  </si>
+  <si>
+    <t>+3 CP when fighting SLOW</t>
+  </si>
+  <si>
+    <t>Lasso</t>
+  </si>
+  <si>
+    <t>Javelin</t>
+  </si>
+  <si>
+    <t>-3 creature CP when targeted</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Mirmillio</t>
+  </si>
+  <si>
+    <t>An amazon from Africa Nova, born to fight.</t>
+  </si>
+  <si>
+    <t>This former legionary is a vetern of a hundred arena fights.</t>
+  </si>
+  <si>
+    <t>This Greek gladiatrix often fights alongside her sister Iomene.</t>
+  </si>
+  <si>
+    <t>This Greek gladiatrix often fights alongside her sister Kephissa.</t>
+  </si>
+  <si>
+    <t>Slow and heavily armoured.</t>
+  </si>
+  <si>
+    <t>Marcus</t>
+  </si>
+  <si>
+    <t>Didius</t>
+  </si>
+  <si>
+    <t>Falco</t>
+  </si>
+  <si>
+    <t>Strabo</t>
+  </si>
+  <si>
+    <t>Ptah</t>
+  </si>
+  <si>
+    <t>An Eqyptian spearman, captured in battle</t>
+  </si>
+  <si>
+    <t>A Gaul held as hostage, sold when her husband was defeated.</t>
+  </si>
+  <si>
+    <t>Casina</t>
+  </si>
+  <si>
+    <t>Hyperion</t>
+  </si>
+  <si>
+    <t>Willibald</t>
+  </si>
+  <si>
+    <t>Gaul</t>
+  </si>
+  <si>
+    <t>Helinand</t>
+  </si>
+  <si>
+    <t>Cossus</t>
+  </si>
+  <si>
+    <t>Lampus</t>
+  </si>
+  <si>
+    <t>Once a Greek poet, who fell into debt.</t>
+  </si>
+  <si>
+    <t>Ubaid</t>
+  </si>
+  <si>
+    <t>An egyptian farmer, in the wrong place at the wrong time.</t>
+  </si>
+  <si>
+    <t>Stadius</t>
+  </si>
+  <si>
+    <t>This mounted soldier takes a little too much pleasure in his task.</t>
+  </si>
+  <si>
+    <t>Aos</t>
+  </si>
+  <si>
+    <t>The exact origins of this Parthian soldier are unknown</t>
+  </si>
+  <si>
+    <t>Bigelis</t>
+  </si>
+  <si>
+    <t>A Gaul who fought in the legions, but betrayed his officer for love.</t>
+  </si>
+  <si>
+    <t>Trajan</t>
+  </si>
+  <si>
+    <t>-8 creature CP when fighting with another Traex</t>
+  </si>
+  <si>
+    <t>Decius</t>
+  </si>
+  <si>
+    <t>Tettidius</t>
+  </si>
+  <si>
+    <t>Trebellius</t>
+  </si>
+  <si>
+    <t>Favonious</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>+2 CP against packs</t>
+  </si>
+  <si>
+    <t>+1 CP against large</t>
+  </si>
+  <si>
+    <t>+2 CP against large</t>
+  </si>
+  <si>
+    <t>After attack, inflict SLOW</t>
+  </si>
+  <si>
+    <t>(TODO) +3 creature CP when fighting with Kephissa</t>
+  </si>
+  <si>
+    <t>-3 creature CP
+(TODO) -5 when with Iomene</t>
+  </si>
+  <si>
     <t>-5 creature CP
--8 when with Mirmillo</t>
-  </si>
-  <si>
-    <t>-3 creature CP
--5 when with Iomene</t>
-  </si>
-  <si>
-    <t>Short Sword</t>
-  </si>
-  <si>
-    <t>Equite</t>
-  </si>
-  <si>
-    <t>+5 CP when fighting SLOW</t>
-  </si>
-  <si>
-    <t>+3 CP when fighting SLOW</t>
-  </si>
-  <si>
-    <t>Lasso</t>
-  </si>
-  <si>
-    <t>Javelin</t>
-  </si>
-  <si>
-    <t>-3 creature CP when targeted</t>
-  </si>
-  <si>
-    <t>Shield</t>
-  </si>
-  <si>
-    <t>Mirmillio</t>
-  </si>
-  <si>
-    <t>An amazon from Africa Nova, born to fight.</t>
-  </si>
-  <si>
-    <t>This former legionary is a vetern of a hundred arena fights.</t>
-  </si>
-  <si>
-    <t>This Greek gladiatrix often fights alongside her sister Iomene.</t>
-  </si>
-  <si>
-    <t>This Greek gladiatrix often fights alongside her sister Kephissa.</t>
-  </si>
-  <si>
-    <t>Slow and heavily armoured.</t>
-  </si>
-  <si>
-    <t>Marcus</t>
-  </si>
-  <si>
-    <t>Didius</t>
-  </si>
-  <si>
-    <t>Falco</t>
-  </si>
-  <si>
-    <t>Strabo</t>
-  </si>
-  <si>
-    <t>Ptah</t>
-  </si>
-  <si>
-    <t>An Eqyptian spearman, captured in battle</t>
-  </si>
-  <si>
-    <t>A Gaul held as hostage, sold when her husband was defeated.</t>
-  </si>
-  <si>
-    <t>Casina</t>
-  </si>
-  <si>
-    <t>Hyperion</t>
-  </si>
-  <si>
-    <t>Willibald</t>
-  </si>
-  <si>
-    <t>Gaul</t>
-  </si>
-  <si>
-    <t>Helinand</t>
-  </si>
-  <si>
-    <t>Cossus</t>
-  </si>
-  <si>
-    <t>Lampus</t>
-  </si>
-  <si>
-    <t>Once a Greek poet, who fell into debt.</t>
-  </si>
-  <si>
-    <t>Ubaid</t>
-  </si>
-  <si>
-    <t>An egyptian farmer, in the wrong place at the wrong time.</t>
-  </si>
-  <si>
-    <t>Stadius</t>
-  </si>
-  <si>
-    <t>This mounted soldier takes a little too much pleasure in his task.</t>
-  </si>
-  <si>
-    <t>Aos</t>
-  </si>
-  <si>
-    <t>The exact origins of this Parthian soldier are unknown</t>
-  </si>
-  <si>
-    <t>Bigelis</t>
-  </si>
-  <si>
-    <t>A Gaul who fought in the legions, but betrayed his officer for love.</t>
-  </si>
-  <si>
-    <t>Trajan</t>
-  </si>
-  <si>
-    <t>-8 creature CP when fighting with another Traex</t>
-  </si>
-  <si>
-    <t>Decius</t>
-  </si>
-  <si>
-    <t>Tettidius</t>
-  </si>
-  <si>
-    <t>Trebellius</t>
-  </si>
-  <si>
-    <t>Favonious</t>
-  </si>
-  <si>
-    <t>img</t>
+(TODO) -8 when with Mirmillo</t>
+  </si>
+  <si>
+    <t>-5 creature CP
+Armoured</t>
+  </si>
+  <si>
+    <t>-6 creature CP
+Armoured</t>
+  </si>
+  <si>
+    <t>-7 creature CP
+Armoured</t>
+  </si>
+  <si>
+    <t>+2 Player Popularity per fight
++4 CP vs players</t>
+  </si>
+  <si>
+    <t>Excitement</t>
   </si>
 </sst>
 </file>
@@ -448,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -456,6 +472,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,10 +758,10 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A50" sqref="A50:XFD59"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +780,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -773,7 +792,7 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F1" t="s">
         <v>7</v>
@@ -782,24 +801,24 @@
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
@@ -817,21 +836,21 @@
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" t="s">
         <v>31</v>
-      </c>
-      <c r="J2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>2</v>
@@ -849,21 +868,21 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
@@ -881,21 +900,21 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
@@ -913,27 +932,27 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -945,27 +964,27 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -977,53 +996,53 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
-        <v>34</v>
-      </c>
       <c r="J8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>2</v>
@@ -1041,21 +1060,21 @@
         <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -1073,21 +1092,21 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
         <v>2</v>
@@ -1105,28 +1124,28 @@
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
-        <v>15</v>
-      </c>
       <c r="F12">
         <v>2</v>
       </c>
@@ -1137,21 +1156,21 @@
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
         <v>2</v>
@@ -1169,21 +1188,21 @@
         <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
         <v>2</v>
@@ -1201,21 +1220,21 @@
         <v>4</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
         <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
       </c>
       <c r="D15" t="s">
         <v>2</v>
@@ -1233,21 +1252,21 @@
         <v>4</v>
       </c>
       <c r="I15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
         <v>2</v>
@@ -1264,16 +1283,19 @@
       <c r="H16">
         <v>4</v>
       </c>
+      <c r="J16" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D17" t="s">
         <v>2</v>
@@ -1290,16 +1312,19 @@
       <c r="H17">
         <v>4</v>
       </c>
+      <c r="J17" s="4" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
         <v>2</v>
@@ -1317,24 +1342,27 @@
         <v>4</v>
       </c>
       <c r="I18" t="s">
-        <v>100</v>
+        <v>92</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s">
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F19">
         <v>5</v>
@@ -1345,19 +1373,19 @@
       <c r="H19">
         <v>4</v>
       </c>
-      <c r="I19" t="s">
-        <v>101</v>
+      <c r="J19" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
         <v>2</v>
@@ -1374,22 +1402,25 @@
       <c r="H20">
         <v>4</v>
       </c>
+      <c r="J20" s="4" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F21">
         <v>5</v>
@@ -1400,16 +1431,22 @@
       <c r="H21">
         <v>4</v>
       </c>
+      <c r="I21" t="s">
+        <v>93</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
         <v>2</v>
@@ -1426,16 +1463,19 @@
       <c r="H22">
         <v>4</v>
       </c>
+      <c r="J22" s="4" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
         <v>2</v>
@@ -1455,19 +1495,19 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F24">
         <v>7</v>
@@ -1481,13 +1521,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
         <v>2</v>
@@ -1505,18 +1545,21 @@
         <v>7</v>
       </c>
       <c r="I25" t="s">
-        <v>111</v>
+        <v>103</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
         <v>2</v>
@@ -1531,24 +1574,24 @@
         <v>3</v>
       </c>
       <c r="H26">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I26" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
         <v>2</v>
@@ -1563,21 +1606,21 @@
         <v>3</v>
       </c>
       <c r="H27">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D28" t="s">
         <v>2</v>
@@ -1592,24 +1635,24 @@
         <v>3</v>
       </c>
       <c r="H28">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I28" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
         <v>2</v>
@@ -1627,24 +1670,24 @@
         <v>7</v>
       </c>
       <c r="I29" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s">
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F30">
         <v>6</v>
@@ -1656,27 +1699,27 @@
         <v>8</v>
       </c>
       <c r="I30" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D31" t="s">
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F31">
         <v>6</v>
@@ -1688,21 +1731,21 @@
         <v>8</v>
       </c>
       <c r="I31" t="s">
-        <v>92</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D32" t="s">
         <v>2</v>
@@ -1720,18 +1763,18 @@
         <v>7</v>
       </c>
       <c r="I32" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D33" t="s">
         <v>2</v>
@@ -1746,24 +1789,24 @@
         <v>3</v>
       </c>
       <c r="H33">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I33" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C34" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D34" t="s">
         <v>2</v>
@@ -1781,18 +1824,18 @@
         <v>8</v>
       </c>
       <c r="I34" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D35" t="s">
         <v>2</v>
@@ -1807,21 +1850,21 @@
         <v>4</v>
       </c>
       <c r="H35">
-        <v>8</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D36" t="s">
         <v>2</v>
@@ -1836,30 +1879,30 @@
         <v>4</v>
       </c>
       <c r="H36">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I36" t="s">
-        <v>109</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="D37" t="s">
         <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F37">
         <v>8</v>
@@ -1868,53 +1911,53 @@
         <v>4</v>
       </c>
       <c r="H37">
-        <v>8</v>
-      </c>
-      <c r="I37" t="s">
-        <v>90</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>62</v>
+        <v>10</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D38" t="s">
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F38">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G38">
         <v>4</v>
       </c>
       <c r="H38">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="I38" t="s">
+        <v>82</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D39" t="s">
         <v>2</v>
@@ -1932,21 +1975,21 @@
         <v>10</v>
       </c>
       <c r="I39" t="s">
-        <v>94</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D40" t="s">
         <v>2</v>
@@ -1961,24 +2004,24 @@
         <v>4</v>
       </c>
       <c r="H40">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I40" t="s">
-        <v>94</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C41" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D41" t="s">
         <v>2</v>
@@ -1993,24 +2036,24 @@
         <v>4</v>
       </c>
       <c r="H41">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I41" t="s">
-        <v>94</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D42" t="s">
         <v>2</v>
@@ -2028,30 +2071,30 @@
         <v>14</v>
       </c>
       <c r="I42" t="s">
-        <v>94</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>76</v>
+        <v>86</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D43" t="s">
         <v>2</v>
       </c>
       <c r="E43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F43">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G43">
         <v>5</v>
@@ -2059,16 +2102,19 @@
       <c r="H43">
         <v>12</v>
       </c>
+      <c r="J43" s="4" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C44" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D44" t="s">
         <v>2</v>
@@ -2077,7 +2123,7 @@
         <v>6</v>
       </c>
       <c r="F44">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G44">
         <v>5</v>
@@ -2086,18 +2132,18 @@
         <v>12</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D45" t="s">
         <v>2</v>
@@ -2106,7 +2152,7 @@
         <v>6</v>
       </c>
       <c r="F45">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G45">
         <v>5</v>
@@ -2115,18 +2161,18 @@
         <v>12</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D46" t="s">
         <v>2</v>
@@ -2135,7 +2181,7 @@
         <v>6</v>
       </c>
       <c r="F46">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G46">
         <v>5</v>
@@ -2144,24 +2190,24 @@
         <v>12</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
         <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F47">
         <v>12</v>
@@ -2173,18 +2219,18 @@
         <v>14</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C48" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D48" t="s">
         <v>2</v>
@@ -2202,18 +2248,18 @@
         <v>14</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" t="s">
         <v>19</v>
-      </c>
-      <c r="C49" t="s">
-        <v>20</v>
       </c>
       <c r="D49" t="s">
         <v>2</v>
@@ -2231,10 +2277,10 @@
         <v>15</v>
       </c>
       <c r="I49" t="s">
-        <v>67</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>